<commit_message>
Inclusão dos Requisitos do sistema
</commit_message>
<xml_diff>
--- a/Requisitos.xlsx
+++ b/Requisitos.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\area de trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\PIM\AnaliseDeRequisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" tabRatio="911" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" tabRatio="911" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Gerais" sheetId="1" r:id="rId1"/>
@@ -516,6 +516,30 @@
     <t>Condomínio deve conter os seguintes atributos Nome(1), Endereço(1), Quantidade de blocos(1), Quantidade de Unidades(1), Data de inauguração(1), Proprietário do condomínio(1) e CNPJ(1)</t>
   </si>
   <si>
+    <t>Todo Terceiro cadastrado deve conter Nome, RG, CNPJ, Nome da empresa, Tipo de serviço prestado e Pelo menos um Telefone</t>
+  </si>
+  <si>
+    <t>Unidade deve conter os seguintes atributos Identificação(1),Proprietário(1), Bloco(1), Quantidades De veiculo(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Todo parâmetro que envolva senha no sistema devera ter uma mascara escondendo os caracteres </t>
+  </si>
+  <si>
+    <t>Cada login de usuário deverá ser único e intransferível</t>
+  </si>
+  <si>
+    <t>Visualização das Visitantes pode ser realizada por todos os usuários.</t>
+  </si>
+  <si>
+    <t>Usuários com acesso de nível Pessoal só podem ver as Visitantes relacionadas a sua própria unidade</t>
+  </si>
+  <si>
+    <t>Todo registro de Visitante devem conter Nome e Rg.</t>
+  </si>
+  <si>
+    <t>Todo registro que for Removido necessariamente deverá ser mantido em um histórico no sistema</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Terceiros  deve conter os seguintes atributos </t>
     </r>
@@ -536,32 +560,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, Tipo de serviço prestado(1), Nome(1), Rg(1), CNPJ(1),  Telefone (5) e Endereço (3)</t>
+      <t>, Tipo de serviço prestado(1), Nome(1), Rg(1), CPF(1),  Telefone (5) e Endereço (3)</t>
     </r>
-  </si>
-  <si>
-    <t>Todo Terceiro cadastrado deve conter Nome, RG, CNPJ, Nome da empresa, Tipo de serviço prestado e Pelo menos um Telefone</t>
-  </si>
-  <si>
-    <t>Unidade deve conter os seguintes atributos Identificação(1),Proprietário(1), Bloco(1), Quantidades De veiculo(1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Todo parâmetro que envolva senha no sistema devera ter uma mascara escondendo os caracteres </t>
-  </si>
-  <si>
-    <t>Cada login de usuário deverá ser único e intransferível</t>
-  </si>
-  <si>
-    <t>Visualização das Visitantes pode ser realizada por todos os usuários.</t>
-  </si>
-  <si>
-    <t>Usuários com acesso de nível Pessoal só podem ver as Visitantes relacionadas a sua própria unidade</t>
-  </si>
-  <si>
-    <t>Todo registro de Visitante devem conter Nome e Rg.</t>
-  </si>
-  <si>
-    <t>Todo registro que for Removido necessariamente deverá ser mantido em um histórico no sistema</t>
   </si>
 </sst>
 </file>
@@ -637,7 +637,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -919,17 +919,6 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1075,13 +1064,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1108,8 +1097,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2350,7 +2339,7 @@
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="20"/>
       <c r="C5" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D5" s="19" t="s">
         <v>6</v>
@@ -2409,7 +2398,7 @@
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" s="20"/>
       <c r="C10" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D10" s="19" t="s">
         <v>6</v>
@@ -2427,7 +2416,7 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="21"/>
       <c r="C12" s="19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>6</v>
@@ -2497,24 +2486,24 @@
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="51"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="52"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="51"/>
-      <c r="C21" s="52"/>
-      <c r="D21" s="52"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="51"/>
     </row>
     <row r="22" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="51"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="52"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="51"/>
     </row>
     <row r="23" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="51"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
       <c r="F23" s="56" t="s">
         <v>11</v>
       </c>
@@ -2522,9 +2511,9 @@
       <c r="H23" s="58"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="51"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="51"/>
       <c r="F24" s="53" t="s">
         <v>7</v>
       </c>
@@ -2537,9 +2526,9 @@
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="51"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="52"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="51"/>
       <c r="F25" s="54"/>
       <c r="G25" s="1" t="s">
         <v>4</v>
@@ -2550,9 +2539,9 @@
       </c>
     </row>
     <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="51"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="52"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="51"/>
       <c r="F26" s="55"/>
       <c r="G26" s="13" t="s">
         <v>12</v>
@@ -2563,9 +2552,9 @@
       </c>
     </row>
     <row r="27" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="51"/>
-      <c r="C27" s="52"/>
-      <c r="D27" s="52"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
       <c r="F27" s="53" t="s">
         <v>3</v>
       </c>
@@ -2578,9 +2567,9 @@
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="51"/>
-      <c r="C28" s="52"/>
-      <c r="D28" s="52"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="51"/>
       <c r="F28" s="54"/>
       <c r="G28" s="1" t="s">
         <v>4</v>
@@ -2591,9 +2580,9 @@
       </c>
     </row>
     <row r="29" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="51"/>
-      <c r="C29" s="52"/>
-      <c r="D29" s="52"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
       <c r="F29" s="55"/>
       <c r="G29" s="16" t="s">
         <v>12</v>
@@ -2604,9 +2593,9 @@
       </c>
     </row>
     <row r="30" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="51"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
       <c r="F30" s="53" t="s">
         <v>8</v>
       </c>
@@ -2619,17 +2608,17 @@
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="51"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
       <c r="F31" s="54"/>
       <c r="G31" s="14"/>
       <c r="H31" s="15"/>
     </row>
     <row r="32" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="51"/>
-      <c r="C32" s="52"/>
-      <c r="D32" s="52"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="51"/>
       <c r="F32" s="54"/>
       <c r="G32" s="1" t="s">
         <v>4</v>
@@ -2640,9 +2629,9 @@
       </c>
     </row>
     <row r="33" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="51"/>
-      <c r="C33" s="52"/>
-      <c r="D33" s="52"/>
+      <c r="B33" s="50"/>
+      <c r="C33" s="51"/>
+      <c r="D33" s="51"/>
       <c r="F33" s="55"/>
       <c r="G33" s="13" t="s">
         <v>12</v>
@@ -2653,1269 +2642,1269 @@
       </c>
     </row>
     <row r="34" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="51"/>
-      <c r="C34" s="52"/>
-      <c r="D34" s="52"/>
+      <c r="B34" s="50"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="51"/>
     </row>
     <row r="35" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="51"/>
-      <c r="C35" s="52"/>
-      <c r="D35" s="52"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="51"/>
+      <c r="D35" s="51"/>
     </row>
     <row r="36" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="51"/>
-      <c r="C36" s="52"/>
-      <c r="D36" s="52"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="51"/>
+      <c r="D36" s="51"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="51"/>
-      <c r="C37" s="52"/>
-      <c r="D37" s="52"/>
+      <c r="B37" s="50"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="51"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="51"/>
-      <c r="C38" s="52"/>
-      <c r="D38" s="52"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="51"/>
+      <c r="D38" s="51"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="51"/>
-      <c r="C39" s="52"/>
-      <c r="D39" s="52"/>
+      <c r="B39" s="50"/>
+      <c r="C39" s="51"/>
+      <c r="D39" s="51"/>
     </row>
     <row r="40" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="51"/>
-      <c r="C40" s="52"/>
-      <c r="D40" s="52"/>
+      <c r="B40" s="50"/>
+      <c r="C40" s="51"/>
+      <c r="D40" s="51"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="51"/>
-      <c r="C41" s="52"/>
-      <c r="D41" s="52"/>
+      <c r="B41" s="50"/>
+      <c r="C41" s="51"/>
+      <c r="D41" s="51"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="51"/>
-      <c r="C42" s="52"/>
-      <c r="D42" s="52"/>
+      <c r="B42" s="50"/>
+      <c r="C42" s="51"/>
+      <c r="D42" s="51"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="51"/>
-      <c r="C43" s="52"/>
-      <c r="D43" s="52"/>
+      <c r="B43" s="50"/>
+      <c r="C43" s="51"/>
+      <c r="D43" s="51"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="51"/>
-      <c r="C44" s="52"/>
-      <c r="D44" s="52"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="51"/>
+      <c r="D44" s="51"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="51"/>
-      <c r="C45" s="52"/>
-      <c r="D45" s="52"/>
+      <c r="B45" s="50"/>
+      <c r="C45" s="51"/>
+      <c r="D45" s="51"/>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="51"/>
-      <c r="C46" s="52"/>
-      <c r="D46" s="52"/>
+      <c r="B46" s="50"/>
+      <c r="C46" s="51"/>
+      <c r="D46" s="51"/>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="51"/>
-      <c r="C47" s="52"/>
-      <c r="D47" s="52"/>
+      <c r="B47" s="50"/>
+      <c r="C47" s="51"/>
+      <c r="D47" s="51"/>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B48" s="51"/>
-      <c r="C48" s="52"/>
-      <c r="D48" s="52"/>
+      <c r="B48" s="50"/>
+      <c r="C48" s="51"/>
+      <c r="D48" s="51"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="51"/>
-      <c r="C49" s="52"/>
-      <c r="D49" s="52"/>
+      <c r="B49" s="50"/>
+      <c r="C49" s="51"/>
+      <c r="D49" s="51"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="51"/>
-      <c r="C50" s="52"/>
-      <c r="D50" s="52"/>
+      <c r="B50" s="50"/>
+      <c r="C50" s="51"/>
+      <c r="D50" s="51"/>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="51"/>
-      <c r="C51" s="52"/>
-      <c r="D51" s="52"/>
+      <c r="B51" s="50"/>
+      <c r="C51" s="51"/>
+      <c r="D51" s="51"/>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="51"/>
-      <c r="C52" s="52"/>
-      <c r="D52" s="52"/>
+      <c r="B52" s="50"/>
+      <c r="C52" s="51"/>
+      <c r="D52" s="51"/>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="51"/>
-      <c r="C53" s="52"/>
-      <c r="D53" s="52"/>
+      <c r="B53" s="50"/>
+      <c r="C53" s="51"/>
+      <c r="D53" s="51"/>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="51"/>
-      <c r="C54" s="52"/>
-      <c r="D54" s="52"/>
+      <c r="B54" s="50"/>
+      <c r="C54" s="51"/>
+      <c r="D54" s="51"/>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="51"/>
-      <c r="C55" s="52"/>
-      <c r="D55" s="52"/>
+      <c r="B55" s="50"/>
+      <c r="C55" s="51"/>
+      <c r="D55" s="51"/>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="51"/>
-      <c r="C56" s="52"/>
-      <c r="D56" s="52"/>
+      <c r="B56" s="50"/>
+      <c r="C56" s="51"/>
+      <c r="D56" s="51"/>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="51"/>
-      <c r="C57" s="52"/>
-      <c r="D57" s="52"/>
+      <c r="B57" s="50"/>
+      <c r="C57" s="51"/>
+      <c r="D57" s="51"/>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="51"/>
-      <c r="C58" s="52"/>
-      <c r="D58" s="52"/>
+      <c r="B58" s="50"/>
+      <c r="C58" s="51"/>
+      <c r="D58" s="51"/>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B59" s="51"/>
-      <c r="C59" s="52"/>
-      <c r="D59" s="52"/>
+      <c r="B59" s="50"/>
+      <c r="C59" s="51"/>
+      <c r="D59" s="51"/>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B60" s="51"/>
-      <c r="C60" s="52"/>
-      <c r="D60" s="52"/>
+      <c r="B60" s="50"/>
+      <c r="C60" s="51"/>
+      <c r="D60" s="51"/>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B61" s="51"/>
-      <c r="C61" s="52"/>
-      <c r="D61" s="52"/>
+      <c r="B61" s="50"/>
+      <c r="C61" s="51"/>
+      <c r="D61" s="51"/>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B62" s="51"/>
-      <c r="C62" s="52"/>
-      <c r="D62" s="52"/>
+      <c r="B62" s="50"/>
+      <c r="C62" s="51"/>
+      <c r="D62" s="51"/>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="51"/>
-      <c r="C63" s="52"/>
-      <c r="D63" s="52"/>
+      <c r="B63" s="50"/>
+      <c r="C63" s="51"/>
+      <c r="D63" s="51"/>
     </row>
     <row r="64" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="51"/>
-      <c r="C64" s="52"/>
-      <c r="D64" s="52"/>
+      <c r="B64" s="50"/>
+      <c r="C64" s="51"/>
+      <c r="D64" s="51"/>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="51"/>
-      <c r="C65" s="52"/>
-      <c r="D65" s="52"/>
+      <c r="B65" s="50"/>
+      <c r="C65" s="51"/>
+      <c r="D65" s="51"/>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B66" s="51"/>
-      <c r="C66" s="52"/>
-      <c r="D66" s="52"/>
+      <c r="B66" s="50"/>
+      <c r="C66" s="51"/>
+      <c r="D66" s="51"/>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="51"/>
-      <c r="C67" s="52"/>
-      <c r="D67" s="52"/>
+      <c r="B67" s="50"/>
+      <c r="C67" s="51"/>
+      <c r="D67" s="51"/>
     </row>
     <row r="68" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="51"/>
-      <c r="C68" s="52"/>
-      <c r="D68" s="52"/>
+      <c r="B68" s="50"/>
+      <c r="C68" s="51"/>
+      <c r="D68" s="51"/>
     </row>
     <row r="69" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="51"/>
-      <c r="C69" s="52"/>
-      <c r="D69" s="52"/>
+      <c r="B69" s="50"/>
+      <c r="C69" s="51"/>
+      <c r="D69" s="51"/>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B70" s="51"/>
-      <c r="C70" s="52"/>
-      <c r="D70" s="52"/>
+      <c r="B70" s="50"/>
+      <c r="C70" s="51"/>
+      <c r="D70" s="51"/>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="51"/>
-      <c r="C71" s="52"/>
-      <c r="D71" s="52"/>
+      <c r="B71" s="50"/>
+      <c r="C71" s="51"/>
+      <c r="D71" s="51"/>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B72" s="51"/>
-      <c r="C72" s="52"/>
-      <c r="D72" s="52"/>
+      <c r="B72" s="50"/>
+      <c r="C72" s="51"/>
+      <c r="D72" s="51"/>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="51"/>
-      <c r="C73" s="52"/>
-      <c r="D73" s="52"/>
+      <c r="B73" s="50"/>
+      <c r="C73" s="51"/>
+      <c r="D73" s="51"/>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B74" s="51"/>
-      <c r="C74" s="52"/>
-      <c r="D74" s="52"/>
+      <c r="B74" s="50"/>
+      <c r="C74" s="51"/>
+      <c r="D74" s="51"/>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="51"/>
-      <c r="C75" s="52"/>
-      <c r="D75" s="52"/>
+      <c r="B75" s="50"/>
+      <c r="C75" s="51"/>
+      <c r="D75" s="51"/>
     </row>
     <row r="76" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="51"/>
-      <c r="C76" s="52"/>
-      <c r="D76" s="52"/>
+      <c r="B76" s="50"/>
+      <c r="C76" s="51"/>
+      <c r="D76" s="51"/>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B77" s="51"/>
-      <c r="C77" s="52"/>
-      <c r="D77" s="52"/>
+      <c r="B77" s="50"/>
+      <c r="C77" s="51"/>
+      <c r="D77" s="51"/>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B78" s="51"/>
-      <c r="C78" s="52"/>
-      <c r="D78" s="52"/>
+      <c r="B78" s="50"/>
+      <c r="C78" s="51"/>
+      <c r="D78" s="51"/>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B79" s="51"/>
-      <c r="C79" s="52"/>
-      <c r="D79" s="52"/>
+      <c r="B79" s="50"/>
+      <c r="C79" s="51"/>
+      <c r="D79" s="51"/>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B80" s="51"/>
-      <c r="C80" s="52"/>
-      <c r="D80" s="52"/>
+      <c r="B80" s="50"/>
+      <c r="C80" s="51"/>
+      <c r="D80" s="51"/>
     </row>
     <row r="81" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="51"/>
-      <c r="C81" s="52"/>
-      <c r="D81" s="52"/>
+      <c r="B81" s="50"/>
+      <c r="C81" s="51"/>
+      <c r="D81" s="51"/>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B82" s="51"/>
-      <c r="C82" s="52"/>
-      <c r="D82" s="52"/>
+      <c r="B82" s="50"/>
+      <c r="C82" s="51"/>
+      <c r="D82" s="51"/>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B83" s="51"/>
-      <c r="C83" s="52"/>
-      <c r="D83" s="52"/>
+      <c r="B83" s="50"/>
+      <c r="C83" s="51"/>
+      <c r="D83" s="51"/>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B84" s="51"/>
-      <c r="C84" s="52"/>
-      <c r="D84" s="52"/>
+      <c r="B84" s="50"/>
+      <c r="C84" s="51"/>
+      <c r="D84" s="51"/>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B85" s="51"/>
-      <c r="C85" s="52"/>
-      <c r="D85" s="52"/>
+      <c r="B85" s="50"/>
+      <c r="C85" s="51"/>
+      <c r="D85" s="51"/>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B86" s="51"/>
-      <c r="C86" s="52"/>
-      <c r="D86" s="52"/>
+      <c r="B86" s="50"/>
+      <c r="C86" s="51"/>
+      <c r="D86" s="51"/>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B87" s="51"/>
-      <c r="C87" s="52"/>
-      <c r="D87" s="52"/>
+      <c r="B87" s="50"/>
+      <c r="C87" s="51"/>
+      <c r="D87" s="51"/>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B88" s="51"/>
-      <c r="C88" s="52"/>
-      <c r="D88" s="52"/>
+      <c r="B88" s="50"/>
+      <c r="C88" s="51"/>
+      <c r="D88" s="51"/>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B89" s="51"/>
-      <c r="C89" s="52"/>
-      <c r="D89" s="52"/>
+      <c r="B89" s="50"/>
+      <c r="C89" s="51"/>
+      <c r="D89" s="51"/>
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B90" s="51"/>
-      <c r="C90" s="52"/>
-      <c r="D90" s="52"/>
+      <c r="B90" s="50"/>
+      <c r="C90" s="51"/>
+      <c r="D90" s="51"/>
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B91" s="51"/>
-      <c r="C91" s="52"/>
-      <c r="D91" s="52"/>
+      <c r="B91" s="50"/>
+      <c r="C91" s="51"/>
+      <c r="D91" s="51"/>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B92" s="51"/>
-      <c r="C92" s="52"/>
-      <c r="D92" s="52"/>
+      <c r="B92" s="50"/>
+      <c r="C92" s="51"/>
+      <c r="D92" s="51"/>
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B93" s="51"/>
-      <c r="C93" s="52"/>
-      <c r="D93" s="52"/>
+      <c r="B93" s="50"/>
+      <c r="C93" s="51"/>
+      <c r="D93" s="51"/>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B94" s="51"/>
-      <c r="C94" s="52"/>
-      <c r="D94" s="52"/>
+      <c r="B94" s="50"/>
+      <c r="C94" s="51"/>
+      <c r="D94" s="51"/>
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B95" s="51"/>
-      <c r="C95" s="52"/>
-      <c r="D95" s="52"/>
+      <c r="B95" s="50"/>
+      <c r="C95" s="51"/>
+      <c r="D95" s="51"/>
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B96" s="51"/>
-      <c r="C96" s="52"/>
-      <c r="D96" s="52"/>
+      <c r="B96" s="50"/>
+      <c r="C96" s="51"/>
+      <c r="D96" s="51"/>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B97" s="51"/>
-      <c r="C97" s="52"/>
-      <c r="D97" s="52"/>
+      <c r="B97" s="50"/>
+      <c r="C97" s="51"/>
+      <c r="D97" s="51"/>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B98" s="51"/>
-      <c r="C98" s="52"/>
-      <c r="D98" s="52"/>
+      <c r="B98" s="50"/>
+      <c r="C98" s="51"/>
+      <c r="D98" s="51"/>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B99" s="51"/>
-      <c r="C99" s="52"/>
-      <c r="D99" s="52"/>
+      <c r="B99" s="50"/>
+      <c r="C99" s="51"/>
+      <c r="D99" s="51"/>
     </row>
     <row r="100" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="51"/>
-      <c r="C100" s="52"/>
-      <c r="D100" s="52"/>
+      <c r="B100" s="50"/>
+      <c r="C100" s="51"/>
+      <c r="D100" s="51"/>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B101" s="51"/>
-      <c r="C101" s="52"/>
-      <c r="D101" s="52"/>
+      <c r="B101" s="50"/>
+      <c r="C101" s="51"/>
+      <c r="D101" s="51"/>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B102" s="51"/>
-      <c r="C102" s="52"/>
-      <c r="D102" s="52"/>
+      <c r="B102" s="50"/>
+      <c r="C102" s="51"/>
+      <c r="D102" s="51"/>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B103" s="51"/>
-      <c r="C103" s="52"/>
-      <c r="D103" s="52"/>
+      <c r="B103" s="50"/>
+      <c r="C103" s="51"/>
+      <c r="D103" s="51"/>
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B104" s="51"/>
-      <c r="C104" s="52"/>
-      <c r="D104" s="52"/>
+      <c r="B104" s="50"/>
+      <c r="C104" s="51"/>
+      <c r="D104" s="51"/>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B105" s="51"/>
-      <c r="C105" s="52"/>
-      <c r="D105" s="52"/>
+      <c r="B105" s="50"/>
+      <c r="C105" s="51"/>
+      <c r="D105" s="51"/>
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B106" s="51"/>
-      <c r="C106" s="52"/>
-      <c r="D106" s="52"/>
+      <c r="B106" s="50"/>
+      <c r="C106" s="51"/>
+      <c r="D106" s="51"/>
     </row>
     <row r="107" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B107" s="51"/>
-      <c r="C107" s="52"/>
-      <c r="D107" s="52"/>
+      <c r="B107" s="50"/>
+      <c r="C107" s="51"/>
+      <c r="D107" s="51"/>
     </row>
     <row r="108" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B108" s="51"/>
-      <c r="C108" s="52"/>
-      <c r="D108" s="52"/>
+      <c r="B108" s="50"/>
+      <c r="C108" s="51"/>
+      <c r="D108" s="51"/>
     </row>
     <row r="109" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B109" s="51"/>
-      <c r="C109" s="52"/>
-      <c r="D109" s="52"/>
+      <c r="B109" s="50"/>
+      <c r="C109" s="51"/>
+      <c r="D109" s="51"/>
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B110" s="51"/>
-      <c r="C110" s="52"/>
-      <c r="D110" s="52"/>
+      <c r="B110" s="50"/>
+      <c r="C110" s="51"/>
+      <c r="D110" s="51"/>
     </row>
     <row r="111" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B111" s="51"/>
-      <c r="C111" s="52"/>
-      <c r="D111" s="52"/>
+      <c r="B111" s="50"/>
+      <c r="C111" s="51"/>
+      <c r="D111" s="51"/>
     </row>
     <row r="112" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B112" s="51"/>
-      <c r="C112" s="52"/>
-      <c r="D112" s="52"/>
+      <c r="B112" s="50"/>
+      <c r="C112" s="51"/>
+      <c r="D112" s="51"/>
     </row>
     <row r="113" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B113" s="51"/>
-      <c r="C113" s="52"/>
-      <c r="D113" s="52"/>
+      <c r="B113" s="50"/>
+      <c r="C113" s="51"/>
+      <c r="D113" s="51"/>
     </row>
     <row r="114" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B114" s="51"/>
-      <c r="C114" s="52"/>
-      <c r="D114" s="52"/>
+      <c r="B114" s="50"/>
+      <c r="C114" s="51"/>
+      <c r="D114" s="51"/>
     </row>
     <row r="115" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B115" s="51"/>
-      <c r="C115" s="52"/>
-      <c r="D115" s="52"/>
+      <c r="B115" s="50"/>
+      <c r="C115" s="51"/>
+      <c r="D115" s="51"/>
     </row>
     <row r="116" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B116" s="51"/>
-      <c r="C116" s="52"/>
-      <c r="D116" s="52"/>
+      <c r="B116" s="50"/>
+      <c r="C116" s="51"/>
+      <c r="D116" s="51"/>
     </row>
     <row r="117" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B117" s="51"/>
-      <c r="C117" s="52"/>
-      <c r="D117" s="52"/>
+      <c r="B117" s="50"/>
+      <c r="C117" s="51"/>
+      <c r="D117" s="51"/>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B118" s="51"/>
-      <c r="C118" s="52"/>
-      <c r="D118" s="52"/>
+      <c r="B118" s="50"/>
+      <c r="C118" s="51"/>
+      <c r="D118" s="51"/>
     </row>
     <row r="119" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B119" s="51"/>
-      <c r="C119" s="52"/>
-      <c r="D119" s="52"/>
+      <c r="B119" s="50"/>
+      <c r="C119" s="51"/>
+      <c r="D119" s="51"/>
     </row>
     <row r="120" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B120" s="51"/>
-      <c r="C120" s="52"/>
-      <c r="D120" s="52"/>
+      <c r="B120" s="50"/>
+      <c r="C120" s="51"/>
+      <c r="D120" s="51"/>
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B121" s="51"/>
-      <c r="C121" s="52"/>
-      <c r="D121" s="52"/>
+      <c r="B121" s="50"/>
+      <c r="C121" s="51"/>
+      <c r="D121" s="51"/>
     </row>
     <row r="122" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B122" s="51"/>
-      <c r="C122" s="52"/>
-      <c r="D122" s="52"/>
+      <c r="B122" s="50"/>
+      <c r="C122" s="51"/>
+      <c r="D122" s="51"/>
     </row>
     <row r="123" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B123" s="51"/>
-      <c r="C123" s="52"/>
-      <c r="D123" s="52"/>
+      <c r="B123" s="50"/>
+      <c r="C123" s="51"/>
+      <c r="D123" s="51"/>
     </row>
     <row r="124" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B124" s="51"/>
-      <c r="C124" s="52"/>
-      <c r="D124" s="52"/>
+      <c r="B124" s="50"/>
+      <c r="C124" s="51"/>
+      <c r="D124" s="51"/>
     </row>
     <row r="125" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B125" s="51"/>
-      <c r="C125" s="52"/>
-      <c r="D125" s="52"/>
+      <c r="B125" s="50"/>
+      <c r="C125" s="51"/>
+      <c r="D125" s="51"/>
     </row>
     <row r="126" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B126" s="51"/>
-      <c r="C126" s="52"/>
-      <c r="D126" s="52"/>
+      <c r="B126" s="50"/>
+      <c r="C126" s="51"/>
+      <c r="D126" s="51"/>
     </row>
     <row r="127" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B127" s="51"/>
-      <c r="C127" s="52"/>
-      <c r="D127" s="52"/>
+      <c r="B127" s="50"/>
+      <c r="C127" s="51"/>
+      <c r="D127" s="51"/>
     </row>
     <row r="128" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B128" s="51"/>
-      <c r="C128" s="52"/>
-      <c r="D128" s="52"/>
+      <c r="B128" s="50"/>
+      <c r="C128" s="51"/>
+      <c r="D128" s="51"/>
     </row>
     <row r="129" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B129" s="51"/>
-      <c r="C129" s="52"/>
-      <c r="D129" s="52"/>
+      <c r="B129" s="50"/>
+      <c r="C129" s="51"/>
+      <c r="D129" s="51"/>
     </row>
     <row r="130" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B130" s="51"/>
-      <c r="C130" s="52"/>
-      <c r="D130" s="52"/>
+      <c r="B130" s="50"/>
+      <c r="C130" s="51"/>
+      <c r="D130" s="51"/>
     </row>
     <row r="131" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B131" s="51"/>
-      <c r="C131" s="52"/>
-      <c r="D131" s="52"/>
+      <c r="B131" s="50"/>
+      <c r="C131" s="51"/>
+      <c r="D131" s="51"/>
     </row>
     <row r="132" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B132" s="51"/>
-      <c r="C132" s="52"/>
-      <c r="D132" s="52"/>
+      <c r="B132" s="50"/>
+      <c r="C132" s="51"/>
+      <c r="D132" s="51"/>
     </row>
     <row r="133" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B133" s="51"/>
-      <c r="C133" s="52"/>
-      <c r="D133" s="52"/>
+      <c r="B133" s="50"/>
+      <c r="C133" s="51"/>
+      <c r="D133" s="51"/>
     </row>
     <row r="134" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B134" s="51"/>
-      <c r="C134" s="52"/>
-      <c r="D134" s="52"/>
+      <c r="B134" s="50"/>
+      <c r="C134" s="51"/>
+      <c r="D134" s="51"/>
     </row>
     <row r="135" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B135" s="51"/>
-      <c r="C135" s="52"/>
-      <c r="D135" s="52"/>
+      <c r="B135" s="50"/>
+      <c r="C135" s="51"/>
+      <c r="D135" s="51"/>
     </row>
     <row r="136" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B136" s="51"/>
-      <c r="C136" s="52"/>
-      <c r="D136" s="52"/>
+      <c r="B136" s="50"/>
+      <c r="C136" s="51"/>
+      <c r="D136" s="51"/>
     </row>
     <row r="137" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B137" s="51"/>
-      <c r="C137" s="52"/>
-      <c r="D137" s="52"/>
+      <c r="B137" s="50"/>
+      <c r="C137" s="51"/>
+      <c r="D137" s="51"/>
     </row>
     <row r="138" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B138" s="51"/>
-      <c r="C138" s="52"/>
-      <c r="D138" s="52"/>
+      <c r="B138" s="50"/>
+      <c r="C138" s="51"/>
+      <c r="D138" s="51"/>
     </row>
     <row r="139" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B139" s="51"/>
-      <c r="C139" s="52"/>
-      <c r="D139" s="52"/>
+      <c r="B139" s="50"/>
+      <c r="C139" s="51"/>
+      <c r="D139" s="51"/>
     </row>
     <row r="140" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B140" s="51"/>
-      <c r="C140" s="52"/>
-      <c r="D140" s="52"/>
+      <c r="B140" s="50"/>
+      <c r="C140" s="51"/>
+      <c r="D140" s="51"/>
     </row>
     <row r="141" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B141" s="51"/>
-      <c r="C141" s="52"/>
-      <c r="D141" s="52"/>
+      <c r="B141" s="50"/>
+      <c r="C141" s="51"/>
+      <c r="D141" s="51"/>
     </row>
     <row r="142" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B142" s="51"/>
-      <c r="C142" s="52"/>
-      <c r="D142" s="52"/>
+      <c r="B142" s="50"/>
+      <c r="C142" s="51"/>
+      <c r="D142" s="51"/>
     </row>
     <row r="143" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B143" s="51"/>
-      <c r="C143" s="52"/>
-      <c r="D143" s="52"/>
+      <c r="B143" s="50"/>
+      <c r="C143" s="51"/>
+      <c r="D143" s="51"/>
     </row>
     <row r="144" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B144" s="51"/>
-      <c r="C144" s="52"/>
-      <c r="D144" s="52"/>
+      <c r="B144" s="50"/>
+      <c r="C144" s="51"/>
+      <c r="D144" s="51"/>
     </row>
     <row r="145" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B145" s="51"/>
-      <c r="C145" s="52"/>
-      <c r="D145" s="52"/>
+      <c r="B145" s="50"/>
+      <c r="C145" s="51"/>
+      <c r="D145" s="51"/>
     </row>
     <row r="146" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B146" s="51"/>
-      <c r="C146" s="52"/>
-      <c r="D146" s="52"/>
+      <c r="B146" s="50"/>
+      <c r="C146" s="51"/>
+      <c r="D146" s="51"/>
     </row>
     <row r="147" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B147" s="51"/>
-      <c r="C147" s="52"/>
-      <c r="D147" s="52"/>
+      <c r="B147" s="50"/>
+      <c r="C147" s="51"/>
+      <c r="D147" s="51"/>
     </row>
     <row r="148" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B148" s="51"/>
-      <c r="C148" s="52"/>
-      <c r="D148" s="52"/>
+      <c r="B148" s="50"/>
+      <c r="C148" s="51"/>
+      <c r="D148" s="51"/>
     </row>
     <row r="149" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B149" s="51"/>
-      <c r="C149" s="52"/>
-      <c r="D149" s="52"/>
+      <c r="B149" s="50"/>
+      <c r="C149" s="51"/>
+      <c r="D149" s="51"/>
     </row>
     <row r="150" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B150" s="51"/>
-      <c r="C150" s="52"/>
-      <c r="D150" s="52"/>
+      <c r="B150" s="50"/>
+      <c r="C150" s="51"/>
+      <c r="D150" s="51"/>
     </row>
     <row r="151" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B151" s="51"/>
-      <c r="C151" s="52"/>
-      <c r="D151" s="52"/>
+      <c r="B151" s="50"/>
+      <c r="C151" s="51"/>
+      <c r="D151" s="51"/>
     </row>
     <row r="152" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B152" s="51"/>
-      <c r="C152" s="52"/>
-      <c r="D152" s="52"/>
+      <c r="B152" s="50"/>
+      <c r="C152" s="51"/>
+      <c r="D152" s="51"/>
     </row>
     <row r="153" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B153" s="51"/>
-      <c r="C153" s="52"/>
-      <c r="D153" s="52"/>
+      <c r="B153" s="50"/>
+      <c r="C153" s="51"/>
+      <c r="D153" s="51"/>
     </row>
     <row r="154" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B154" s="51"/>
-      <c r="C154" s="52"/>
-      <c r="D154" s="52"/>
+      <c r="B154" s="50"/>
+      <c r="C154" s="51"/>
+      <c r="D154" s="51"/>
     </row>
     <row r="155" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B155" s="51"/>
-      <c r="C155" s="52"/>
-      <c r="D155" s="52"/>
+      <c r="B155" s="50"/>
+      <c r="C155" s="51"/>
+      <c r="D155" s="51"/>
     </row>
     <row r="156" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B156" s="51"/>
-      <c r="C156" s="52"/>
-      <c r="D156" s="52"/>
+      <c r="B156" s="50"/>
+      <c r="C156" s="51"/>
+      <c r="D156" s="51"/>
     </row>
     <row r="157" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B157" s="51"/>
-      <c r="C157" s="52"/>
-      <c r="D157" s="52"/>
+      <c r="B157" s="50"/>
+      <c r="C157" s="51"/>
+      <c r="D157" s="51"/>
     </row>
     <row r="158" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B158" s="51"/>
-      <c r="C158" s="52"/>
-      <c r="D158" s="52"/>
+      <c r="B158" s="50"/>
+      <c r="C158" s="51"/>
+      <c r="D158" s="51"/>
     </row>
     <row r="159" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B159" s="51"/>
-      <c r="C159" s="52"/>
-      <c r="D159" s="52"/>
+      <c r="B159" s="50"/>
+      <c r="C159" s="51"/>
+      <c r="D159" s="51"/>
     </row>
     <row r="160" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B160" s="51"/>
-      <c r="C160" s="52"/>
-      <c r="D160" s="52"/>
+      <c r="B160" s="50"/>
+      <c r="C160" s="51"/>
+      <c r="D160" s="51"/>
     </row>
     <row r="161" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B161" s="51"/>
-      <c r="C161" s="52"/>
-      <c r="D161" s="52"/>
+      <c r="B161" s="50"/>
+      <c r="C161" s="51"/>
+      <c r="D161" s="51"/>
     </row>
     <row r="162" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B162" s="51"/>
-      <c r="C162" s="52"/>
-      <c r="D162" s="52"/>
+      <c r="B162" s="50"/>
+      <c r="C162" s="51"/>
+      <c r="D162" s="51"/>
     </row>
     <row r="163" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B163" s="51"/>
-      <c r="C163" s="52"/>
-      <c r="D163" s="52"/>
+      <c r="B163" s="50"/>
+      <c r="C163" s="51"/>
+      <c r="D163" s="51"/>
     </row>
     <row r="164" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B164" s="51"/>
-      <c r="C164" s="52"/>
-      <c r="D164" s="52"/>
+      <c r="B164" s="50"/>
+      <c r="C164" s="51"/>
+      <c r="D164" s="51"/>
     </row>
     <row r="165" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B165" s="51"/>
-      <c r="C165" s="52"/>
-      <c r="D165" s="52"/>
+      <c r="B165" s="50"/>
+      <c r="C165" s="51"/>
+      <c r="D165" s="51"/>
     </row>
     <row r="166" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B166" s="51"/>
-      <c r="C166" s="52"/>
-      <c r="D166" s="52"/>
+      <c r="B166" s="50"/>
+      <c r="C166" s="51"/>
+      <c r="D166" s="51"/>
     </row>
     <row r="167" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B167" s="51"/>
-      <c r="C167" s="52"/>
-      <c r="D167" s="52"/>
+      <c r="B167" s="50"/>
+      <c r="C167" s="51"/>
+      <c r="D167" s="51"/>
     </row>
     <row r="168" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B168" s="51"/>
-      <c r="C168" s="52"/>
-      <c r="D168" s="52"/>
+      <c r="B168" s="50"/>
+      <c r="C168" s="51"/>
+      <c r="D168" s="51"/>
     </row>
     <row r="169" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B169" s="51"/>
-      <c r="C169" s="52"/>
-      <c r="D169" s="52"/>
+      <c r="B169" s="50"/>
+      <c r="C169" s="51"/>
+      <c r="D169" s="51"/>
     </row>
     <row r="170" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B170" s="51"/>
-      <c r="C170" s="52"/>
-      <c r="D170" s="52"/>
+      <c r="B170" s="50"/>
+      <c r="C170" s="51"/>
+      <c r="D170" s="51"/>
     </row>
     <row r="171" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B171" s="51"/>
-      <c r="C171" s="52"/>
-      <c r="D171" s="52"/>
+      <c r="B171" s="50"/>
+      <c r="C171" s="51"/>
+      <c r="D171" s="51"/>
     </row>
     <row r="172" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B172" s="51"/>
-      <c r="C172" s="52"/>
-      <c r="D172" s="52"/>
+      <c r="B172" s="50"/>
+      <c r="C172" s="51"/>
+      <c r="D172" s="51"/>
     </row>
     <row r="173" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B173" s="51"/>
-      <c r="C173" s="52"/>
-      <c r="D173" s="52"/>
+      <c r="B173" s="50"/>
+      <c r="C173" s="51"/>
+      <c r="D173" s="51"/>
     </row>
     <row r="174" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B174" s="51"/>
-      <c r="C174" s="52"/>
-      <c r="D174" s="52"/>
+      <c r="B174" s="50"/>
+      <c r="C174" s="51"/>
+      <c r="D174" s="51"/>
     </row>
     <row r="175" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B175" s="51"/>
-      <c r="C175" s="52"/>
-      <c r="D175" s="52"/>
+      <c r="B175" s="50"/>
+      <c r="C175" s="51"/>
+      <c r="D175" s="51"/>
     </row>
     <row r="176" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B176" s="51"/>
-      <c r="C176" s="52"/>
-      <c r="D176" s="52"/>
+      <c r="B176" s="50"/>
+      <c r="C176" s="51"/>
+      <c r="D176" s="51"/>
     </row>
     <row r="177" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B177" s="51"/>
-      <c r="C177" s="52"/>
-      <c r="D177" s="52"/>
+      <c r="B177" s="50"/>
+      <c r="C177" s="51"/>
+      <c r="D177" s="51"/>
     </row>
     <row r="178" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B178" s="51"/>
-      <c r="C178" s="52"/>
-      <c r="D178" s="52"/>
+      <c r="B178" s="50"/>
+      <c r="C178" s="51"/>
+      <c r="D178" s="51"/>
     </row>
     <row r="179" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B179" s="51"/>
-      <c r="C179" s="52"/>
-      <c r="D179" s="52"/>
+      <c r="B179" s="50"/>
+      <c r="C179" s="51"/>
+      <c r="D179" s="51"/>
     </row>
     <row r="180" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B180" s="51"/>
-      <c r="C180" s="52"/>
-      <c r="D180" s="52"/>
+      <c r="B180" s="50"/>
+      <c r="C180" s="51"/>
+      <c r="D180" s="51"/>
     </row>
     <row r="181" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B181" s="51"/>
-      <c r="C181" s="52"/>
-      <c r="D181" s="52"/>
+      <c r="B181" s="50"/>
+      <c r="C181" s="51"/>
+      <c r="D181" s="51"/>
     </row>
     <row r="182" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B182" s="51"/>
-      <c r="C182" s="52"/>
-      <c r="D182" s="52"/>
+      <c r="B182" s="50"/>
+      <c r="C182" s="51"/>
+      <c r="D182" s="51"/>
     </row>
     <row r="183" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B183" s="51"/>
-      <c r="C183" s="52"/>
-      <c r="D183" s="52"/>
+      <c r="B183" s="50"/>
+      <c r="C183" s="51"/>
+      <c r="D183" s="51"/>
     </row>
     <row r="184" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B184" s="51"/>
-      <c r="C184" s="52"/>
-      <c r="D184" s="52"/>
+      <c r="B184" s="50"/>
+      <c r="C184" s="51"/>
+      <c r="D184" s="51"/>
     </row>
     <row r="185" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B185" s="51"/>
-      <c r="C185" s="52"/>
-      <c r="D185" s="52"/>
+      <c r="B185" s="50"/>
+      <c r="C185" s="51"/>
+      <c r="D185" s="51"/>
     </row>
     <row r="186" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B186" s="51"/>
-      <c r="C186" s="52"/>
-      <c r="D186" s="52"/>
+      <c r="B186" s="50"/>
+      <c r="C186" s="51"/>
+      <c r="D186" s="51"/>
     </row>
     <row r="187" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B187" s="51"/>
-      <c r="C187" s="52"/>
-      <c r="D187" s="52"/>
+      <c r="B187" s="50"/>
+      <c r="C187" s="51"/>
+      <c r="D187" s="51"/>
     </row>
     <row r="188" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B188" s="51"/>
-      <c r="C188" s="52"/>
-      <c r="D188" s="52"/>
+      <c r="B188" s="50"/>
+      <c r="C188" s="51"/>
+      <c r="D188" s="51"/>
     </row>
     <row r="189" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B189" s="51"/>
-      <c r="C189" s="52"/>
-      <c r="D189" s="52"/>
+      <c r="B189" s="50"/>
+      <c r="C189" s="51"/>
+      <c r="D189" s="51"/>
     </row>
     <row r="190" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B190" s="51"/>
-      <c r="C190" s="52"/>
-      <c r="D190" s="52"/>
+      <c r="B190" s="50"/>
+      <c r="C190" s="51"/>
+      <c r="D190" s="51"/>
     </row>
     <row r="191" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B191" s="51"/>
-      <c r="C191" s="52"/>
-      <c r="D191" s="52"/>
+      <c r="B191" s="50"/>
+      <c r="C191" s="51"/>
+      <c r="D191" s="51"/>
     </row>
     <row r="192" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B192" s="51"/>
-      <c r="C192" s="52"/>
-      <c r="D192" s="52"/>
+      <c r="B192" s="50"/>
+      <c r="C192" s="51"/>
+      <c r="D192" s="51"/>
     </row>
     <row r="193" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B193" s="51"/>
-      <c r="C193" s="52"/>
-      <c r="D193" s="52"/>
+      <c r="B193" s="50"/>
+      <c r="C193" s="51"/>
+      <c r="D193" s="51"/>
     </row>
     <row r="194" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B194" s="51"/>
-      <c r="C194" s="52"/>
-      <c r="D194" s="52"/>
+      <c r="B194" s="50"/>
+      <c r="C194" s="51"/>
+      <c r="D194" s="51"/>
     </row>
     <row r="195" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B195" s="51"/>
-      <c r="C195" s="52"/>
-      <c r="D195" s="52"/>
+      <c r="B195" s="50"/>
+      <c r="C195" s="51"/>
+      <c r="D195" s="51"/>
     </row>
     <row r="196" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B196" s="51"/>
-      <c r="C196" s="52"/>
-      <c r="D196" s="52"/>
+      <c r="B196" s="50"/>
+      <c r="C196" s="51"/>
+      <c r="D196" s="51"/>
     </row>
     <row r="197" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B197" s="51"/>
-      <c r="C197" s="52"/>
-      <c r="D197" s="52"/>
+      <c r="B197" s="50"/>
+      <c r="C197" s="51"/>
+      <c r="D197" s="51"/>
     </row>
     <row r="198" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B198" s="51"/>
-      <c r="C198" s="52"/>
-      <c r="D198" s="52"/>
+      <c r="B198" s="50"/>
+      <c r="C198" s="51"/>
+      <c r="D198" s="51"/>
     </row>
     <row r="199" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B199" s="51"/>
-      <c r="C199" s="52"/>
-      <c r="D199" s="52"/>
+      <c r="B199" s="50"/>
+      <c r="C199" s="51"/>
+      <c r="D199" s="51"/>
     </row>
     <row r="200" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B200" s="51"/>
-      <c r="C200" s="52"/>
-      <c r="D200" s="52"/>
+      <c r="B200" s="50"/>
+      <c r="C200" s="51"/>
+      <c r="D200" s="51"/>
     </row>
     <row r="201" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B201" s="51"/>
-      <c r="C201" s="52"/>
-      <c r="D201" s="52"/>
+      <c r="B201" s="50"/>
+      <c r="C201" s="51"/>
+      <c r="D201" s="51"/>
     </row>
     <row r="202" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B202" s="51"/>
-      <c r="C202" s="52"/>
-      <c r="D202" s="52"/>
+      <c r="B202" s="50"/>
+      <c r="C202" s="51"/>
+      <c r="D202" s="51"/>
     </row>
     <row r="203" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B203" s="51"/>
-      <c r="C203" s="52"/>
-      <c r="D203" s="52"/>
+      <c r="B203" s="50"/>
+      <c r="C203" s="51"/>
+      <c r="D203" s="51"/>
     </row>
     <row r="204" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B204" s="51"/>
-      <c r="C204" s="52"/>
-      <c r="D204" s="52"/>
+      <c r="B204" s="50"/>
+      <c r="C204" s="51"/>
+      <c r="D204" s="51"/>
     </row>
     <row r="205" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B205" s="51"/>
-      <c r="C205" s="52"/>
-      <c r="D205" s="52"/>
+      <c r="B205" s="50"/>
+      <c r="C205" s="51"/>
+      <c r="D205" s="51"/>
     </row>
     <row r="206" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B206" s="51"/>
-      <c r="C206" s="52"/>
-      <c r="D206" s="52"/>
+      <c r="B206" s="50"/>
+      <c r="C206" s="51"/>
+      <c r="D206" s="51"/>
     </row>
     <row r="207" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B207" s="51"/>
-      <c r="C207" s="52"/>
-      <c r="D207" s="52"/>
+      <c r="B207" s="50"/>
+      <c r="C207" s="51"/>
+      <c r="D207" s="51"/>
     </row>
     <row r="208" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B208" s="51"/>
-      <c r="C208" s="52"/>
-      <c r="D208" s="52"/>
+      <c r="B208" s="50"/>
+      <c r="C208" s="51"/>
+      <c r="D208" s="51"/>
     </row>
     <row r="209" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B209" s="51"/>
-      <c r="C209" s="52"/>
-      <c r="D209" s="52"/>
+      <c r="B209" s="50"/>
+      <c r="C209" s="51"/>
+      <c r="D209" s="51"/>
     </row>
     <row r="210" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B210" s="51"/>
-      <c r="C210" s="52"/>
-      <c r="D210" s="52"/>
+      <c r="B210" s="50"/>
+      <c r="C210" s="51"/>
+      <c r="D210" s="51"/>
     </row>
     <row r="211" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B211" s="51"/>
-      <c r="C211" s="52"/>
-      <c r="D211" s="52"/>
+      <c r="B211" s="50"/>
+      <c r="C211" s="51"/>
+      <c r="D211" s="51"/>
     </row>
     <row r="212" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B212" s="51"/>
-      <c r="C212" s="52"/>
-      <c r="D212" s="52"/>
+      <c r="B212" s="50"/>
+      <c r="C212" s="51"/>
+      <c r="D212" s="51"/>
     </row>
     <row r="213" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B213" s="51"/>
-      <c r="C213" s="52"/>
-      <c r="D213" s="52"/>
+      <c r="B213" s="50"/>
+      <c r="C213" s="51"/>
+      <c r="D213" s="51"/>
     </row>
     <row r="214" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B214" s="51"/>
-      <c r="C214" s="52"/>
-      <c r="D214" s="52"/>
+      <c r="B214" s="50"/>
+      <c r="C214" s="51"/>
+      <c r="D214" s="51"/>
     </row>
     <row r="215" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B215" s="51"/>
-      <c r="C215" s="52"/>
-      <c r="D215" s="52"/>
+      <c r="B215" s="50"/>
+      <c r="C215" s="51"/>
+      <c r="D215" s="51"/>
     </row>
     <row r="216" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B216" s="51"/>
-      <c r="C216" s="52"/>
-      <c r="D216" s="52"/>
+      <c r="B216" s="50"/>
+      <c r="C216" s="51"/>
+      <c r="D216" s="51"/>
     </row>
     <row r="217" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B217" s="51"/>
-      <c r="C217" s="52"/>
-      <c r="D217" s="52"/>
+      <c r="B217" s="50"/>
+      <c r="C217" s="51"/>
+      <c r="D217" s="51"/>
     </row>
     <row r="218" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B218" s="51"/>
-      <c r="C218" s="52"/>
-      <c r="D218" s="52"/>
+      <c r="B218" s="50"/>
+      <c r="C218" s="51"/>
+      <c r="D218" s="51"/>
     </row>
     <row r="219" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B219" s="51"/>
-      <c r="C219" s="52"/>
-      <c r="D219" s="52"/>
+      <c r="B219" s="50"/>
+      <c r="C219" s="51"/>
+      <c r="D219" s="51"/>
     </row>
     <row r="220" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B220" s="51"/>
-      <c r="C220" s="52"/>
-      <c r="D220" s="52"/>
+      <c r="B220" s="50"/>
+      <c r="C220" s="51"/>
+      <c r="D220" s="51"/>
     </row>
     <row r="221" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B221" s="51"/>
-      <c r="C221" s="52"/>
-      <c r="D221" s="52"/>
+      <c r="B221" s="50"/>
+      <c r="C221" s="51"/>
+      <c r="D221" s="51"/>
     </row>
     <row r="222" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B222" s="51"/>
-      <c r="C222" s="52"/>
-      <c r="D222" s="52"/>
+      <c r="B222" s="50"/>
+      <c r="C222" s="51"/>
+      <c r="D222" s="51"/>
     </row>
     <row r="223" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B223" s="51"/>
-      <c r="C223" s="52"/>
-      <c r="D223" s="52"/>
+      <c r="B223" s="50"/>
+      <c r="C223" s="51"/>
+      <c r="D223" s="51"/>
     </row>
     <row r="224" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B224" s="51"/>
-      <c r="C224" s="52"/>
-      <c r="D224" s="52"/>
+      <c r="B224" s="50"/>
+      <c r="C224" s="51"/>
+      <c r="D224" s="51"/>
     </row>
     <row r="225" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B225" s="51"/>
-      <c r="C225" s="52"/>
-      <c r="D225" s="52"/>
+      <c r="B225" s="50"/>
+      <c r="C225" s="51"/>
+      <c r="D225" s="51"/>
     </row>
     <row r="226" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B226" s="51"/>
-      <c r="C226" s="52"/>
-      <c r="D226" s="52"/>
+      <c r="B226" s="50"/>
+      <c r="C226" s="51"/>
+      <c r="D226" s="51"/>
     </row>
     <row r="227" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B227" s="51"/>
-      <c r="C227" s="52"/>
-      <c r="D227" s="52"/>
+      <c r="B227" s="50"/>
+      <c r="C227" s="51"/>
+      <c r="D227" s="51"/>
     </row>
     <row r="228" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B228" s="51"/>
-      <c r="C228" s="52"/>
-      <c r="D228" s="52"/>
+      <c r="B228" s="50"/>
+      <c r="C228" s="51"/>
+      <c r="D228" s="51"/>
     </row>
     <row r="229" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B229" s="51"/>
-      <c r="C229" s="52"/>
-      <c r="D229" s="52"/>
+      <c r="B229" s="50"/>
+      <c r="C229" s="51"/>
+      <c r="D229" s="51"/>
     </row>
     <row r="230" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B230" s="51"/>
-      <c r="C230" s="52"/>
-      <c r="D230" s="52"/>
+      <c r="B230" s="50"/>
+      <c r="C230" s="51"/>
+      <c r="D230" s="51"/>
     </row>
     <row r="231" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B231" s="51"/>
-      <c r="C231" s="52"/>
-      <c r="D231" s="52"/>
+      <c r="B231" s="50"/>
+      <c r="C231" s="51"/>
+      <c r="D231" s="51"/>
     </row>
     <row r="232" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B232" s="51"/>
-      <c r="C232" s="52"/>
-      <c r="D232" s="52"/>
+      <c r="B232" s="50"/>
+      <c r="C232" s="51"/>
+      <c r="D232" s="51"/>
     </row>
     <row r="233" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B233" s="51"/>
-      <c r="C233" s="52"/>
-      <c r="D233" s="52"/>
+      <c r="B233" s="50"/>
+      <c r="C233" s="51"/>
+      <c r="D233" s="51"/>
     </row>
     <row r="234" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B234" s="51"/>
-      <c r="C234" s="52"/>
-      <c r="D234" s="52"/>
+      <c r="B234" s="50"/>
+      <c r="C234" s="51"/>
+      <c r="D234" s="51"/>
     </row>
     <row r="235" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B235" s="51"/>
-      <c r="C235" s="52"/>
-      <c r="D235" s="52"/>
+      <c r="B235" s="50"/>
+      <c r="C235" s="51"/>
+      <c r="D235" s="51"/>
     </row>
     <row r="236" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B236" s="51"/>
-      <c r="C236" s="52"/>
-      <c r="D236" s="52"/>
+      <c r="B236" s="50"/>
+      <c r="C236" s="51"/>
+      <c r="D236" s="51"/>
     </row>
     <row r="237" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B237" s="51"/>
-      <c r="C237" s="52"/>
-      <c r="D237" s="52"/>
+      <c r="B237" s="50"/>
+      <c r="C237" s="51"/>
+      <c r="D237" s="51"/>
     </row>
     <row r="238" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B238" s="51"/>
-      <c r="C238" s="52"/>
-      <c r="D238" s="52"/>
+      <c r="B238" s="50"/>
+      <c r="C238" s="51"/>
+      <c r="D238" s="51"/>
     </row>
     <row r="239" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B239" s="51"/>
-      <c r="C239" s="52"/>
-      <c r="D239" s="52"/>
+      <c r="B239" s="50"/>
+      <c r="C239" s="51"/>
+      <c r="D239" s="51"/>
     </row>
     <row r="240" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B240" s="51"/>
-      <c r="C240" s="52"/>
-      <c r="D240" s="52"/>
+      <c r="B240" s="50"/>
+      <c r="C240" s="51"/>
+      <c r="D240" s="51"/>
     </row>
     <row r="241" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B241" s="51"/>
-      <c r="C241" s="52"/>
-      <c r="D241" s="52"/>
+      <c r="B241" s="50"/>
+      <c r="C241" s="51"/>
+      <c r="D241" s="51"/>
     </row>
     <row r="242" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B242" s="51"/>
-      <c r="C242" s="52"/>
-      <c r="D242" s="52"/>
+      <c r="B242" s="50"/>
+      <c r="C242" s="51"/>
+      <c r="D242" s="51"/>
     </row>
     <row r="243" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B243" s="51"/>
-      <c r="C243" s="52"/>
-      <c r="D243" s="52"/>
+      <c r="B243" s="50"/>
+      <c r="C243" s="51"/>
+      <c r="D243" s="51"/>
     </row>
     <row r="244" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B244" s="51"/>
-      <c r="C244" s="52"/>
-      <c r="D244" s="52"/>
+      <c r="B244" s="50"/>
+      <c r="C244" s="51"/>
+      <c r="D244" s="51"/>
     </row>
     <row r="245" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B245" s="51"/>
-      <c r="C245" s="52"/>
-      <c r="D245" s="52"/>
+      <c r="B245" s="50"/>
+      <c r="C245" s="51"/>
+      <c r="D245" s="51"/>
     </row>
     <row r="246" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B246" s="51"/>
-      <c r="C246" s="52"/>
-      <c r="D246" s="52"/>
+      <c r="B246" s="50"/>
+      <c r="C246" s="51"/>
+      <c r="D246" s="51"/>
     </row>
     <row r="247" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B247" s="51"/>
-      <c r="C247" s="52"/>
-      <c r="D247" s="52"/>
+      <c r="B247" s="50"/>
+      <c r="C247" s="51"/>
+      <c r="D247" s="51"/>
     </row>
     <row r="248" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B248" s="51"/>
-      <c r="C248" s="52"/>
-      <c r="D248" s="52"/>
+      <c r="B248" s="50"/>
+      <c r="C248" s="51"/>
+      <c r="D248" s="51"/>
     </row>
     <row r="249" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B249" s="51"/>
-      <c r="C249" s="52"/>
-      <c r="D249" s="52"/>
+      <c r="B249" s="50"/>
+      <c r="C249" s="51"/>
+      <c r="D249" s="51"/>
     </row>
     <row r="250" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B250" s="51"/>
-      <c r="C250" s="52"/>
-      <c r="D250" s="52"/>
+      <c r="B250" s="50"/>
+      <c r="C250" s="51"/>
+      <c r="D250" s="51"/>
     </row>
     <row r="251" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B251" s="51"/>
-      <c r="C251" s="52"/>
-      <c r="D251" s="52"/>
+      <c r="B251" s="50"/>
+      <c r="C251" s="51"/>
+      <c r="D251" s="51"/>
     </row>
     <row r="252" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B252" s="51"/>
-      <c r="C252" s="52"/>
-      <c r="D252" s="52"/>
+      <c r="B252" s="50"/>
+      <c r="C252" s="51"/>
+      <c r="D252" s="51"/>
     </row>
     <row r="253" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B253" s="51"/>
-      <c r="C253" s="52"/>
-      <c r="D253" s="52"/>
+      <c r="B253" s="50"/>
+      <c r="C253" s="51"/>
+      <c r="D253" s="51"/>
     </row>
     <row r="254" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B254" s="51"/>
-      <c r="C254" s="52"/>
-      <c r="D254" s="52"/>
+      <c r="B254" s="50"/>
+      <c r="C254" s="51"/>
+      <c r="D254" s="51"/>
     </row>
     <row r="255" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B255" s="51"/>
-      <c r="C255" s="52"/>
-      <c r="D255" s="52"/>
+      <c r="B255" s="50"/>
+      <c r="C255" s="51"/>
+      <c r="D255" s="51"/>
     </row>
     <row r="256" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B256" s="51"/>
-      <c r="C256" s="52"/>
-      <c r="D256" s="52"/>
+      <c r="B256" s="50"/>
+      <c r="C256" s="51"/>
+      <c r="D256" s="51"/>
     </row>
     <row r="257" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B257" s="51"/>
-      <c r="C257" s="52"/>
-      <c r="D257" s="52"/>
+      <c r="B257" s="50"/>
+      <c r="C257" s="51"/>
+      <c r="D257" s="51"/>
     </row>
     <row r="258" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B258" s="51"/>
-      <c r="C258" s="52"/>
-      <c r="D258" s="52"/>
+      <c r="B258" s="50"/>
+      <c r="C258" s="51"/>
+      <c r="D258" s="51"/>
     </row>
     <row r="259" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B259" s="51"/>
-      <c r="C259" s="52"/>
-      <c r="D259" s="52"/>
+      <c r="B259" s="50"/>
+      <c r="C259" s="51"/>
+      <c r="D259" s="51"/>
     </row>
     <row r="260" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B260" s="51"/>
-      <c r="C260" s="52"/>
-      <c r="D260" s="52"/>
+      <c r="B260" s="50"/>
+      <c r="C260" s="51"/>
+      <c r="D260" s="51"/>
     </row>
     <row r="261" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B261" s="51"/>
-      <c r="C261" s="52"/>
-      <c r="D261" s="52"/>
+      <c r="B261" s="50"/>
+      <c r="C261" s="51"/>
+      <c r="D261" s="51"/>
     </row>
     <row r="262" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B262" s="51"/>
-      <c r="C262" s="52"/>
-      <c r="D262" s="52"/>
+      <c r="B262" s="50"/>
+      <c r="C262" s="51"/>
+      <c r="D262" s="51"/>
     </row>
     <row r="263" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B263" s="51"/>
-      <c r="C263" s="52"/>
-      <c r="D263" s="52"/>
+      <c r="B263" s="50"/>
+      <c r="C263" s="51"/>
+      <c r="D263" s="51"/>
     </row>
     <row r="264" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B264" s="51"/>
-      <c r="C264" s="52"/>
-      <c r="D264" s="52"/>
+      <c r="B264" s="50"/>
+      <c r="C264" s="51"/>
+      <c r="D264" s="51"/>
     </row>
     <row r="265" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B265" s="51"/>
-      <c r="C265" s="52"/>
-      <c r="D265" s="52"/>
+      <c r="B265" s="50"/>
+      <c r="C265" s="51"/>
+      <c r="D265" s="51"/>
     </row>
     <row r="266" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B266" s="51"/>
-      <c r="C266" s="52"/>
-      <c r="D266" s="52"/>
+      <c r="B266" s="50"/>
+      <c r="C266" s="51"/>
+      <c r="D266" s="51"/>
     </row>
     <row r="267" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B267" s="51"/>
-      <c r="C267" s="52"/>
-      <c r="D267" s="52"/>
+      <c r="B267" s="50"/>
+      <c r="C267" s="51"/>
+      <c r="D267" s="51"/>
     </row>
     <row r="268" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B268" s="51"/>
-      <c r="C268" s="52"/>
-      <c r="D268" s="52"/>
+      <c r="B268" s="50"/>
+      <c r="C268" s="51"/>
+      <c r="D268" s="51"/>
     </row>
     <row r="269" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B269" s="51"/>
-      <c r="C269" s="52"/>
-      <c r="D269" s="52"/>
+      <c r="B269" s="50"/>
+      <c r="C269" s="51"/>
+      <c r="D269" s="51"/>
     </row>
     <row r="270" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B270" s="51"/>
-      <c r="C270" s="52"/>
-      <c r="D270" s="52"/>
+      <c r="B270" s="50"/>
+      <c r="C270" s="51"/>
+      <c r="D270" s="51"/>
     </row>
     <row r="271" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B271" s="51"/>
-      <c r="C271" s="52"/>
-      <c r="D271" s="52"/>
+      <c r="B271" s="50"/>
+      <c r="C271" s="51"/>
+      <c r="D271" s="51"/>
     </row>
     <row r="272" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B272" s="51"/>
-      <c r="C272" s="52"/>
-      <c r="D272" s="52"/>
+      <c r="B272" s="50"/>
+      <c r="C272" s="51"/>
+      <c r="D272" s="51"/>
     </row>
     <row r="273" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B273" s="51"/>
-      <c r="C273" s="52"/>
-      <c r="D273" s="52"/>
+      <c r="B273" s="50"/>
+      <c r="C273" s="51"/>
+      <c r="D273" s="51"/>
     </row>
     <row r="274" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B274" s="51"/>
-      <c r="C274" s="52"/>
-      <c r="D274" s="52"/>
+      <c r="B274" s="50"/>
+      <c r="C274" s="51"/>
+      <c r="D274" s="51"/>
     </row>
     <row r="275" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B275" s="51"/>
-      <c r="C275" s="52"/>
-      <c r="D275" s="52"/>
+      <c r="B275" s="50"/>
+      <c r="C275" s="51"/>
+      <c r="D275" s="51"/>
     </row>
     <row r="276" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B276" s="51"/>
-      <c r="C276" s="52"/>
-      <c r="D276" s="52"/>
+      <c r="B276" s="50"/>
+      <c r="C276" s="51"/>
+      <c r="D276" s="51"/>
     </row>
     <row r="277" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B277" s="51"/>
-      <c r="C277" s="52"/>
-      <c r="D277" s="52"/>
+      <c r="B277" s="50"/>
+      <c r="C277" s="51"/>
+      <c r="D277" s="51"/>
     </row>
     <row r="278" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B278" s="51"/>
-      <c r="C278" s="52"/>
-      <c r="D278" s="52"/>
+      <c r="B278" s="50"/>
+      <c r="C278" s="51"/>
+      <c r="D278" s="51"/>
     </row>
     <row r="279" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B279" s="51"/>
-      <c r="C279" s="52"/>
-      <c r="D279" s="52"/>
+      <c r="B279" s="50"/>
+      <c r="C279" s="51"/>
+      <c r="D279" s="51"/>
     </row>
     <row r="280" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B280" s="51"/>
-      <c r="C280" s="52"/>
-      <c r="D280" s="52"/>
+      <c r="B280" s="50"/>
+      <c r="C280" s="51"/>
+      <c r="D280" s="51"/>
     </row>
     <row r="281" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B281" s="51"/>
-      <c r="C281" s="52"/>
-      <c r="D281" s="52"/>
+      <c r="B281" s="50"/>
+      <c r="C281" s="51"/>
+      <c r="D281" s="51"/>
     </row>
     <row r="282" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B282" s="51"/>
-      <c r="C282" s="52"/>
-      <c r="D282" s="52"/>
+      <c r="B282" s="50"/>
+      <c r="C282" s="51"/>
+      <c r="D282" s="51"/>
     </row>
     <row r="283" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B283" s="51"/>
-      <c r="C283" s="52"/>
-      <c r="D283" s="52"/>
+      <c r="B283" s="50"/>
+      <c r="C283" s="51"/>
+      <c r="D283" s="51"/>
     </row>
     <row r="284" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B284" s="51"/>
-      <c r="C284" s="52"/>
-      <c r="D284" s="52"/>
+      <c r="B284" s="50"/>
+      <c r="C284" s="51"/>
+      <c r="D284" s="51"/>
     </row>
     <row r="285" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B285" s="51"/>
-      <c r="C285" s="52"/>
-      <c r="D285" s="52"/>
+      <c r="B285" s="50"/>
+      <c r="C285" s="51"/>
+      <c r="D285" s="51"/>
     </row>
     <row r="286" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B286" s="51"/>
-      <c r="C286" s="52"/>
-      <c r="D286" s="52"/>
+      <c r="B286" s="50"/>
+      <c r="C286" s="51"/>
+      <c r="D286" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3944,7 +3933,7 @@
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4018,8 +4007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D9"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4349,21 +4338,21 @@
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="34"/>
       <c r="C5" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D5" s="34"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="34"/>
       <c r="C6" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D6" s="34"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="34"/>
       <c r="C7" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D7" s="34"/>
     </row>
@@ -5162,7 +5151,7 @@
   <dimension ref="B2:D12"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5186,7 +5175,7 @@
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="34"/>
       <c r="C3" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D3" s="33" t="s">
         <v>6</v>
@@ -5235,7 +5224,7 @@
       <c r="D9" s="34"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="50"/>
+      <c r="C10" s="61"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C12" s="39"/>
@@ -5255,8 +5244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5343,7 +5332,7 @@
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5409,7 +5398,7 @@
   <dimension ref="B2:D10"/>
   <sheetViews>
     <sheetView zoomScale="113" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5433,7 +5422,7 @@
     <row r="3" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="34"/>
       <c r="C3" s="32" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="D3" s="28" t="s">
         <v>6</v>
@@ -5456,7 +5445,7 @@
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="34"/>
       <c r="C6" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D6" s="34"/>
     </row>
@@ -5482,7 +5471,7 @@
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5550,7 +5539,7 @@
   <dimension ref="B2:D10"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>